<commit_message>
Add session details and log
</commit_message>
<xml_diff>
--- a/lib/assets/templates/template.xlsx
+++ b/lib/assets/templates/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amrit\iCloudDrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5781730A-2653-4D98-9E52-27157220EDBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C7D04E2-BD91-4098-8499-320CE184EAA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Session Length (Hours)</t>
   </si>
@@ -128,6 +128,12 @@
   </si>
   <si>
     <t>Roadway Type</t>
+  </si>
+  <si>
+    <t>Volunteers</t>
+  </si>
+  <si>
+    <t>Amrit Manhas, Greg Pikatis, Alobo Dreok</t>
   </si>
 </sst>
 </file>
@@ -1081,16 +1087,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="20.1875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.4375" customWidth="1"/>
     <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="10.5625" customWidth="1"/>
     <col min="13" max="13" width="19" bestFit="1" customWidth="1"/>
@@ -1300,41 +1306,49 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A13" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A14" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B14" s="3">
         <f>B12*B5</f>
         <v>2.5</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A14" s="9" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A15" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-    </row>
-    <row r="16" spans="1:9" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="14" t="s">
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+    </row>
+    <row r="17" spans="1:3" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="14"/>
-    </row>
-    <row r="17" spans="1:3" ht="16.149999999999999" thickTop="1" x14ac:dyDescent="0.5"/>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A18" s="1"/>
-    </row>
+      <c r="B17" s="14"/>
+    </row>
+    <row r="18" spans="1:3" ht="16.149999999999999" thickTop="1" x14ac:dyDescent="0.5"/>
     <row r="19" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="C19" s="2"/>
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="C20" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:I1"/>
-    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix time and styling
</commit_message>
<xml_diff>
--- a/lib/assets/templates/template.xlsx
+++ b/lib/assets/templates/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amrit\iCloudDrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C7D04E2-BD91-4098-8499-320CE184EAA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F4FB4A-0173-4156-8DA6-E77A01A7CE23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>Session Length (Hours)</t>
   </si>
@@ -134,6 +134,15 @@
   </si>
   <si>
     <t>Amrit Manhas, Greg Pikatis, Alobo Dreok</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Volunteer</t>
+  </si>
+  <si>
+    <t>Speed Range</t>
   </si>
 </sst>
 </file>
@@ -292,7 +301,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -472,8 +481,20 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -617,19 +638,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -641,14 +649,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -696,41 +706,56 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="5" xfId="10" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="6" borderId="5" xfId="10" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="12" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" xfId="10" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="11" xfId="21" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="12" borderId="10" xfId="21" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="13" xfId="21" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="12" xfId="21" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="12" borderId="11" xfId="21" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="14" xfId="21" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="10" xfId="21" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="10" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="6" borderId="10" xfId="10" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="13" xfId="19" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="10" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="5" xfId="39" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="5" xfId="31" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="5" xfId="19" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="34" borderId="5" xfId="19" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="5" xfId="19" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="5" xfId="21" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -779,6 +804,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFBDBD"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1087,17 +1117,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="20.1875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.4375" customWidth="1"/>
-    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="4" width="20.5625" customWidth="1"/>
     <col min="5" max="8" width="10.5625" customWidth="1"/>
     <col min="13" max="13" width="19" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19.5" bestFit="1" customWidth="1"/>
@@ -1108,53 +1136,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="D1" s="14" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" ht="16.149999999999999" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="C2" s="9"/>
+      <c r="D2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="11">
         <v>44687.420138888891</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="C3" s="11"/>
+      <c r="D3" s="12" t="s">
         <v>20</v>
       </c>
       <c r="E3" s="3">
@@ -1169,16 +1200,19 @@
       <c r="H3" s="3">
         <v>0</v>
       </c>
-      <c r="I3" s="7"/>
+      <c r="I3" s="18">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="11">
         <v>44687.503472222219</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="C4" s="11"/>
+      <c r="D4" s="12" t="s">
         <v>21</v>
       </c>
       <c r="E4" s="3">
@@ -1193,16 +1227,19 @@
       <c r="H4" s="3">
         <v>0</v>
       </c>
-      <c r="I4" s="7"/>
+      <c r="I4" s="18">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A5" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="3">
+      <c r="A5" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="9">
         <v>1.25</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="C5" s="9"/>
+      <c r="D5" s="12" t="s">
         <v>22</v>
       </c>
       <c r="E5" s="3">
@@ -1217,16 +1254,19 @@
       <c r="H5" s="3">
         <v>0</v>
       </c>
-      <c r="I5" s="7"/>
+      <c r="I5" s="18">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="9">
         <v>30</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="C6" s="9"/>
+      <c r="D6" s="12" t="s">
         <v>23</v>
       </c>
       <c r="E6" s="3">
@@ -1241,114 +1281,160 @@
       <c r="H6" s="3">
         <v>0</v>
       </c>
-      <c r="I6" s="7"/>
+      <c r="I6" s="18">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="C7" s="9"/>
+      <c r="D7" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
+      <c r="E7" s="14">
+        <v>10</v>
+      </c>
+      <c r="F7" s="15">
+        <v>10</v>
+      </c>
+      <c r="G7" s="16">
+        <v>10</v>
+      </c>
+      <c r="H7" s="17">
+        <v>10</v>
+      </c>
+      <c r="I7" s="19">
+        <v>10</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="9" t="s">
         <v>11</v>
       </c>
+      <c r="C8" s="9"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="9" t="s">
         <v>12</v>
       </c>
+      <c r="C9" s="9"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="9" t="s">
         <v>13</v>
       </c>
+      <c r="C10" s="9"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="9">
         <v>2</v>
       </c>
+      <c r="C12" s="9"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="9" t="s">
         <v>33</v>
       </c>
+      <c r="C13" s="9"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="9">
         <f>B12*B5</f>
         <v>2.5</v>
       </c>
+      <c r="C14" s="9"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="3"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-    </row>
-    <row r="17" spans="1:3" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="14" t="s">
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+    </row>
+    <row r="16" spans="1:9" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="14"/>
-    </row>
-    <row r="18" spans="1:3" ht="16.149999999999999" thickTop="1" x14ac:dyDescent="0.5"/>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="C20" s="2"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+    </row>
+    <row r="17" spans="1:4" ht="16.149999999999999" thickTop="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A18" s="1"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="C19" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:B1"/>
+  <mergeCells count="17">
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:I1"/>
-    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed template line border
</commit_message>
<xml_diff>
--- a/lib/assets/templates/template.xlsx
+++ b/lib/assets/templates/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amrit\iCloudDrive\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rahim/Desktop/5_week_project_course/speedwatch/lib/assets/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AAECADF-ABD9-48DF-A7BD-8A15B38DD12A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727172DD-819B-A240-958A-88EF894F7901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,14 +32,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
   <si>
     <t>Session Length (Hours)</t>
   </si>
   <si>
-    <t>Speed Limit</t>
-  </si>
-  <si>
     <t>Traffic Direction</t>
   </si>
   <si>
@@ -122,6 +119,12 @@
   </si>
   <si>
     <t>Speed Range</t>
+  </si>
+  <si>
+    <t>Speed Limit (km/h)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -473,7 +476,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -644,33 +647,9 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="thick">
         <color theme="4"/>
       </top>
@@ -681,12 +660,8 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thick">
-        <color theme="4"/>
-      </top>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -737,7 +712,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -755,15 +730,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="12" borderId="10" xfId="21" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="13" xfId="19" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="11" borderId="10" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="5" xfId="39" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="5" xfId="31" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -779,29 +748,38 @@
     <xf numFmtId="0" fontId="16" fillId="12" borderId="5" xfId="21" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="10" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="14" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="10" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="6" borderId="10" xfId="10" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="13" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="15" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="13" xfId="39" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="10" xfId="19" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="6" borderId="14" xfId="10" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="6" borderId="15" xfId="10" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="16" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="17" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="14" xfId="21" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1166,244 +1144,263 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:C8"/>
+      <selection activeCell="A16" sqref="A16:D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="20.5625" customWidth="1"/>
-    <col min="5" max="8" width="10.5625" customWidth="1"/>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
+    <col min="2" max="2" width="41.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="20.5" customWidth="1"/>
+    <col min="5" max="8" width="10.5" customWidth="1"/>
     <col min="13" max="13" width="19" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.1875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.3125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.3125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-    </row>
-    <row r="2" spans="1:9" ht="16.149999999999999" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="5" t="s">
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+    </row>
+    <row r="2" spans="1:9" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="16"/>
+      <c r="C2" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="17"/>
+      <c r="C3" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A3" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="21"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
-      <c r="I3" s="15"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A4" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="3"/>
+      <c r="I3" s="13"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="17"/>
+      <c r="C4" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="21"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
-      <c r="I4" s="15"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A5" s="10" t="s">
+      <c r="I4" s="13"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="3"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="21"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-      <c r="I5" s="15"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A6" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="3"/>
+      <c r="I5" s="13"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="16"/>
+      <c r="C6" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="21"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
-      <c r="I6" s="15"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A7" s="10" t="s">
+      <c r="I6" s="13"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="16"/>
+      <c r="C7" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="22"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="14"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="16"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A8" s="10" t="s">
+      <c r="B8" s="16"/>
+      <c r="C8" s="19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="16"/>
+      <c r="C9" s="19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="20"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A9" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="20"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A10" s="10" t="s">
+      <c r="B10" s="16"/>
+      <c r="C10" s="19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="20"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A11" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="20"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="19" t="s">
+        <v>30</v>
+      </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A12" s="10" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="16"/>
+      <c r="C12" s="19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="16"/>
+      <c r="C13" s="19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="20"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A13" s="10" t="s">
+      <c r="B14" s="16"/>
+      <c r="C14" s="19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="16"/>
+      <c r="C15" s="19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+    </row>
+    <row r="17" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="20"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A14" s="10" t="s">
+      <c r="B17" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="20"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A15" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-    </row>
-    <row r="16" spans="1:9" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-    </row>
-    <row r="17" spans="1:4" ht="16.149999999999999" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="8" t="s">
+      <c r="D17" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.5">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C19" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B12:C12"/>
+  <mergeCells count="3">
+    <mergeCell ref="A1:B1"/>
     <mergeCell ref="A16:D16"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:I1"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- Fixed LARGETRUCK to LargeTruck in output - Removed Unused imports
</commit_message>
<xml_diff>
--- a/lib/assets/templates/template.xlsx
+++ b/lib/assets/templates/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rahim/Desktop/5_week_project_course/speedwatch/lib/assets/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727172DD-819B-A240-958A-88EF894F7901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D1ACFA6-9E7E-CE49-8E32-FCB08AC7B7EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -476,7 +476,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -653,15 +653,6 @@
       <top style="thick">
         <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -712,7 +703,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -748,9 +739,6 @@
     <xf numFmtId="0" fontId="16" fillId="12" borderId="5" xfId="21" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="10" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -778,7 +766,7 @@
     <xf numFmtId="0" fontId="16" fillId="12" borderId="14" xfId="21" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1144,15 +1132,15 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:D16"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.5" customWidth="1"/>
     <col min="2" max="2" width="41.1640625" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="20.5" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="10.5" customWidth="1"/>
     <col min="13" max="13" width="19" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19.5" bestFit="1" customWidth="1"/>
@@ -1163,31 +1151,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="15" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
     </row>
     <row r="2" spans="1:9" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="24" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="23" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="5" t="s">
@@ -1210,14 +1198,14 @@
       <c r="A3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="23" t="s">
+      <c r="B3" s="16"/>
+      <c r="C3" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="21"/>
+      <c r="E3" s="20"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -1227,14 +1215,14 @@
       <c r="A4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="23" t="s">
+      <c r="B4" s="16"/>
+      <c r="C4" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="21"/>
+      <c r="E4" s="20"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -1244,14 +1232,14 @@
       <c r="A5" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="23" t="s">
+      <c r="B5" s="15"/>
+      <c r="C5" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="21"/>
+      <c r="E5" s="20"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -1261,14 +1249,14 @@
       <c r="A6" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="23" t="s">
+      <c r="B6" s="15"/>
+      <c r="C6" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="21"/>
+      <c r="E6" s="20"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -1278,14 +1266,14 @@
       <c r="A7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="23" t="s">
+      <c r="B7" s="15"/>
+      <c r="C7" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="22"/>
+      <c r="E7" s="21"/>
       <c r="F7" s="10"/>
       <c r="G7" s="11"/>
       <c r="H7" s="12"/>
@@ -1295,8 +1283,8 @@
       <c r="A8" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="19" t="s">
+      <c r="B8" s="15"/>
+      <c r="C8" s="18" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1304,8 +1292,8 @@
       <c r="A9" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="19" t="s">
+      <c r="B9" s="15"/>
+      <c r="C9" s="18" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1313,8 +1301,8 @@
       <c r="A10" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="19" t="s">
+      <c r="B10" s="15"/>
+      <c r="C10" s="18" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1322,8 +1310,8 @@
       <c r="A11" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="19" t="s">
+      <c r="B11" s="15"/>
+      <c r="C11" s="18" t="s">
         <v>30</v>
       </c>
       <c r="D11" s="7"/>
@@ -1336,8 +1324,8 @@
       <c r="A12" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="19" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="18" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1345,8 +1333,8 @@
       <c r="A13" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="19" t="s">
+      <c r="B13" s="15"/>
+      <c r="C13" s="18" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1354,8 +1342,8 @@
       <c r="A14" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="19" t="s">
+      <c r="B14" s="15"/>
+      <c r="C14" s="18" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1363,18 +1351,18 @@
       <c r="A15" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="19" t="s">
+      <c r="B15" s="15"/>
+      <c r="C15" s="18" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
     </row>
     <row r="17" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">

</xml_diff>